<commit_message>
Dopolnjeni podatki + poizvedba za splošno regato
</commit_message>
<xml_diff>
--- a/podatki/Koper/Koper_jadralci.xlsx
+++ b/podatki/Koper/Koper_jadralci.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Koper_jadralci" sheetId="1" r:id="rId1"/>
+    <sheet name="List1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="274">
   <si>
     <t>SLO711</t>
   </si>
@@ -835,6 +836,12 @@
   </si>
   <si>
     <t>Sara Ratoša</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSERT INTO clanstvo(klub_idklub,tekmovalec_idtekmovalec) </t>
+  </si>
+  <si>
+    <t>SELECT k.idklub, t.idtekmovalec FROM (</t>
   </si>
 </sst>
 </file>
@@ -1665,8 +1672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" activeCellId="1" sqref="C1:C1048576 K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6006,4 +6013,3119 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G119"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E119"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" t="str">
+        <f t="shared" ref="C1:C64" si="0">CONCATENATE(" SELECT idklub FROM klub WHERE ime = '",G1,"') k, (")</f>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D1" t="str">
+        <f t="shared" ref="D1:D64" si="1">CONCATENATE(" SELECT idtekmovalec FROM tekmovalec WHERE sailno = '",F1,"') t")</f>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO711') t</v>
+      </c>
+      <c r="E1" t="str">
+        <f t="shared" ref="E1:E64" si="2">CONCATENATE(" WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = '",F1,"');")</f>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO711');</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO922') t</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO922');</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'KYCK') k, (</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'AUT1053') t</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'AUT1053');</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK IZOLA') k, (</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO255') t</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO255');</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BYC') k, (</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN918') t</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN918');</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'WSA') k, (</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'AUT1205') t</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'AUT1205');</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK IZOLA') k, (</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO1212') t</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO1212');</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>272</v>
+      </c>
+      <c r="B8" t="s">
+        <v>273</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SPARTACUS YC') k, (</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN2005') t</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN2005');</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SPARTACUS YC') k, (</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN1331') t</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN1331');</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BYC') k, (</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN1327') t</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN1327');</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>272</v>
+      </c>
+      <c r="B11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK PIRAT') k, (</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO750') t</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO750');</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>272</v>
+      </c>
+      <c r="B12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SPARTACUS YC') k, (</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN1379') t</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN1379');</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>272</v>
+      </c>
+      <c r="B13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'KYCK') k, (</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'AUT1188') t</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'AUT1188');</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>272</v>
+      </c>
+      <c r="B14" t="s">
+        <v>273</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO811') t</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO811');</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>272</v>
+      </c>
+      <c r="B15" t="s">
+        <v>273</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO944') t</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO944');</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>272</v>
+      </c>
+      <c r="B16" t="s">
+        <v>273</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SPARTACUS YC') k, (</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN1343') t</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN1343');</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>272</v>
+      </c>
+      <c r="B17" t="s">
+        <v>273</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK IZOLA') k, (</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO228') t</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO228');</v>
+      </c>
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>272</v>
+      </c>
+      <c r="B18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK PIRAT') k, (</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO64') t</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO64');</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>272</v>
+      </c>
+      <c r="B19" t="s">
+        <v>273</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BYC') k, (</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN901') t</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN901');</v>
+      </c>
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>272</v>
+      </c>
+      <c r="B20" t="s">
+        <v>273</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK PIRAT') k, (</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO1005') t</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO1005');</v>
+      </c>
+      <c r="F20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>272</v>
+      </c>
+      <c r="B21" t="s">
+        <v>273</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BYC') k, (</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN909') t</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN909');</v>
+      </c>
+      <c r="F21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>272</v>
+      </c>
+      <c r="B22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SVBG') k, (</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA7621') t</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA7621');</v>
+      </c>
+      <c r="F22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>272</v>
+      </c>
+      <c r="B23" t="s">
+        <v>273</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BYC') k, (</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN1313') t</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN1313');</v>
+      </c>
+      <c r="F23" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>272</v>
+      </c>
+      <c r="B24" t="s">
+        <v>273</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'KEREKED SAILING CLUB') k, (</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN704') t</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN704');</v>
+      </c>
+      <c r="F24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>272</v>
+      </c>
+      <c r="B25" t="s">
+        <v>273</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SPARTACUS YC') k, (</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN58') t</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN58');</v>
+      </c>
+      <c r="F25" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B26" t="s">
+        <v>273</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BYC 1912') k, (</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN1912') t</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN1912');</v>
+      </c>
+      <c r="F26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>272</v>
+      </c>
+      <c r="B27" t="s">
+        <v>273</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK BURJA IZOLA') k, (</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO311') t</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO311');</v>
+      </c>
+      <c r="F27" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>272</v>
+      </c>
+      <c r="B28" t="s">
+        <v>273</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK PIRAT') k, (</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO758') t</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO758');</v>
+      </c>
+      <c r="F28" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>272</v>
+      </c>
+      <c r="B29" t="s">
+        <v>273</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO952') t</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO952');</v>
+      </c>
+      <c r="F29" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>272</v>
+      </c>
+      <c r="B30" t="s">
+        <v>273</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'WSC CRNOMELJ') k, (</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO234') t</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO234');</v>
+      </c>
+      <c r="F30" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>272</v>
+      </c>
+      <c r="B31" t="s">
+        <v>273</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SCTWV ACHENSEE') k, (</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'AUT1231') t</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'AUT1231');</v>
+      </c>
+      <c r="F31" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>272</v>
+      </c>
+      <c r="B32" t="s">
+        <v>273</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BYC 1912') k, (</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN148') t</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN148');</v>
+      </c>
+      <c r="F32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>272</v>
+      </c>
+      <c r="B33" t="s">
+        <v>273</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SPARTACUS YC') k, (</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN1311') t</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN1311');</v>
+      </c>
+      <c r="F33" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>272</v>
+      </c>
+      <c r="B34" t="s">
+        <v>273</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'KYCK') k, (</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'AUT1255') t</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'AUT1255');</v>
+      </c>
+      <c r="F34" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>272</v>
+      </c>
+      <c r="B35" t="s">
+        <v>273</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK IZOLA') k, (</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO87') t</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO87');</v>
+      </c>
+      <c r="F35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>272</v>
+      </c>
+      <c r="B36" t="s">
+        <v>273</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SPARTACUS YC') k, (</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN1304') t</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN1304');</v>
+      </c>
+      <c r="F36" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>272</v>
+      </c>
+      <c r="B37" t="s">
+        <v>273</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK OLIMPIC') k, (</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO666') t</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO666');</v>
+      </c>
+      <c r="F37" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>272</v>
+      </c>
+      <c r="B38" t="s">
+        <v>273</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'THE YKA') k, (</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN375') t</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN375');</v>
+      </c>
+      <c r="F38" t="s">
+        <v>86</v>
+      </c>
+      <c r="G38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>272</v>
+      </c>
+      <c r="B39" t="s">
+        <v>273</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BYC') k, (</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN1310') t</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN1310');</v>
+      </c>
+      <c r="F39" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>272</v>
+      </c>
+      <c r="B40" t="s">
+        <v>273</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SÉP') k, (</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN238') t</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN238');</v>
+      </c>
+      <c r="F40" t="s">
+        <v>91</v>
+      </c>
+      <c r="G40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>272</v>
+      </c>
+      <c r="B41" t="s">
+        <v>273</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK PIRAT') k, (</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO411') t</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO411');</v>
+      </c>
+      <c r="F41" t="s">
+        <v>94</v>
+      </c>
+      <c r="G41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>272</v>
+      </c>
+      <c r="B42" t="s">
+        <v>273</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO951') t</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO951');</v>
+      </c>
+      <c r="F42" t="s">
+        <v>96</v>
+      </c>
+      <c r="G42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>272</v>
+      </c>
+      <c r="B43" t="s">
+        <v>273</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO956') t</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO956');</v>
+      </c>
+      <c r="F43" t="s">
+        <v>98</v>
+      </c>
+      <c r="G43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>272</v>
+      </c>
+      <c r="B44" t="s">
+        <v>273</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SCTWV') k, (</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'AUT1351') t</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'AUT1351');</v>
+      </c>
+      <c r="F44" t="s">
+        <v>100</v>
+      </c>
+      <c r="G44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>272</v>
+      </c>
+      <c r="B45" t="s">
+        <v>273</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BYC') k, (</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN1337') t</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN1337');</v>
+      </c>
+      <c r="F45" t="s">
+        <v>103</v>
+      </c>
+      <c r="G45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>272</v>
+      </c>
+      <c r="B46" t="s">
+        <v>273</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'WSA') k, (</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'AUT996') t</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'AUT996');</v>
+      </c>
+      <c r="F46" t="s">
+        <v>105</v>
+      </c>
+      <c r="G46" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>272</v>
+      </c>
+      <c r="B47" t="s">
+        <v>273</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO913') t</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO913');</v>
+      </c>
+      <c r="F47" t="s">
+        <v>107</v>
+      </c>
+      <c r="G47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>272</v>
+      </c>
+      <c r="B48" t="s">
+        <v>273</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SVBG') k, (</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA11') t</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA11');</v>
+      </c>
+      <c r="F48" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>272</v>
+      </c>
+      <c r="B49" t="s">
+        <v>273</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK BURJA IZOLA') k, (</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO395') t</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO395');</v>
+      </c>
+      <c r="F49" t="s">
+        <v>111</v>
+      </c>
+      <c r="G49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>272</v>
+      </c>
+      <c r="B50" t="s">
+        <v>273</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SBSK') k, (</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SVK12') t</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SVK12');</v>
+      </c>
+      <c r="F50" t="s">
+        <v>113</v>
+      </c>
+      <c r="G50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>272</v>
+      </c>
+      <c r="B51" t="s">
+        <v>273</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK PIRAT') k, (</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO512') t</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO512');</v>
+      </c>
+      <c r="F51" t="s">
+        <v>116</v>
+      </c>
+      <c r="G51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>272</v>
+      </c>
+      <c r="B52" t="s">
+        <v>273</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK LJUBLJANA') k, (</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO525') t</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO525');</v>
+      </c>
+      <c r="F52" t="s">
+        <v>117</v>
+      </c>
+      <c r="G52" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>272</v>
+      </c>
+      <c r="B53" t="s">
+        <v>273</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'TPK SIRENA') k, (</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA8341') t</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA8341');</v>
+      </c>
+      <c r="F53" t="s">
+        <v>120</v>
+      </c>
+      <c r="G53" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>272</v>
+      </c>
+      <c r="B54" t="s">
+        <v>273</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'THE YKA') k, (</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN950') t</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN950');</v>
+      </c>
+      <c r="F54" t="s">
+        <v>123</v>
+      </c>
+      <c r="G54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>272</v>
+      </c>
+      <c r="B55" t="s">
+        <v>273</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK BURJA IZOLA') k, (</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO377') t</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO377');</v>
+      </c>
+      <c r="F55" t="s">
+        <v>125</v>
+      </c>
+      <c r="G55" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>272</v>
+      </c>
+      <c r="B56" t="s">
+        <v>273</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK IZOLA') k, (</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO189') t</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO189');</v>
+      </c>
+      <c r="F56" t="s">
+        <v>127</v>
+      </c>
+      <c r="G56" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>272</v>
+      </c>
+      <c r="B57" t="s">
+        <v>273</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SÉP') k, (</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN232') t</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN232');</v>
+      </c>
+      <c r="F57" t="s">
+        <v>129</v>
+      </c>
+      <c r="G57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>272</v>
+      </c>
+      <c r="B58" t="s">
+        <v>273</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'KEREKED SAILING CLUB') k, (</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN714') t</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN714');</v>
+      </c>
+      <c r="F58" t="s">
+        <v>131</v>
+      </c>
+      <c r="G58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>272</v>
+      </c>
+      <c r="B59" t="s">
+        <v>273</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SCTWV ACHENSEE') k, (</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'AUT1848') t</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'AUT1848');</v>
+      </c>
+      <c r="F59" t="s">
+        <v>133</v>
+      </c>
+      <c r="G59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>272</v>
+      </c>
+      <c r="B60" t="s">
+        <v>273</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK BURJA IZOLA') k, (</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO372') t</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO372');</v>
+      </c>
+      <c r="F60" t="s">
+        <v>135</v>
+      </c>
+      <c r="G60" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>272</v>
+      </c>
+      <c r="B61" t="s">
+        <v>273</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'THE YKA') k, (</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN372') t</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN372');</v>
+      </c>
+      <c r="F61" t="s">
+        <v>137</v>
+      </c>
+      <c r="G61" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>272</v>
+      </c>
+      <c r="B62" t="s">
+        <v>273</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO111') t</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO111');</v>
+      </c>
+      <c r="F62" t="s">
+        <v>139</v>
+      </c>
+      <c r="G62" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>272</v>
+      </c>
+      <c r="B63" t="s">
+        <v>273</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'TPK SIRENA') k, (</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA6588') t</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA6588');</v>
+      </c>
+      <c r="F63" t="s">
+        <v>141</v>
+      </c>
+      <c r="G63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>272</v>
+      </c>
+      <c r="B64" t="s">
+        <v>273</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BYC') k, (</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN1322') t</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN1322');</v>
+      </c>
+      <c r="F64" t="s">
+        <v>143</v>
+      </c>
+      <c r="G64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>272</v>
+      </c>
+      <c r="B65" t="s">
+        <v>273</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" ref="C65:C119" si="3">CONCATENATE(" SELECT idklub FROM klub WHERE ime = '",G65,"') k, (")</f>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'THE YKA') k, (</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" ref="D65:D119" si="4">CONCATENATE(" SELECT idtekmovalec FROM tekmovalec WHERE sailno = '",F65,"') t")</f>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN12944') t</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" ref="E65:E119" si="5">CONCATENATE(" WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = '",F65,"');")</f>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN12944');</v>
+      </c>
+      <c r="F65" t="s">
+        <v>145</v>
+      </c>
+      <c r="G65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>272</v>
+      </c>
+      <c r="B66" t="s">
+        <v>273</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'THE YKA') k, (</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN12946') t</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN12946');</v>
+      </c>
+      <c r="F66" t="s">
+        <v>147</v>
+      </c>
+      <c r="G66" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>272</v>
+      </c>
+      <c r="B67" t="s">
+        <v>273</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK OLIMPIC') k, (</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO631') t</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO631');</v>
+      </c>
+      <c r="F67" t="s">
+        <v>149</v>
+      </c>
+      <c r="G67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>272</v>
+      </c>
+      <c r="B68" t="s">
+        <v>273</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO511') t</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO511');</v>
+      </c>
+      <c r="F68" t="s">
+        <v>151</v>
+      </c>
+      <c r="G68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>272</v>
+      </c>
+      <c r="B69" t="s">
+        <v>273</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK OLIMPIC') k, (</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO677') t</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO677');</v>
+      </c>
+      <c r="F69" t="s">
+        <v>153</v>
+      </c>
+      <c r="G69" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>272</v>
+      </c>
+      <c r="B70" t="s">
+        <v>273</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SVBG') k, (</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA8308') t</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA8308');</v>
+      </c>
+      <c r="F70" t="s">
+        <v>155</v>
+      </c>
+      <c r="G70" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>272</v>
+      </c>
+      <c r="B71" t="s">
+        <v>273</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'TJ LANKROUN') k, (</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'CZE829') t</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'CZE829');</v>
+      </c>
+      <c r="F71" t="s">
+        <v>157</v>
+      </c>
+      <c r="G71" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>272</v>
+      </c>
+      <c r="B72" t="s">
+        <v>273</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SMD PIRAN') k, (</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO875') t</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO875');</v>
+      </c>
+      <c r="F72" t="s">
+        <v>160</v>
+      </c>
+      <c r="G72" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>272</v>
+      </c>
+      <c r="B73" t="s">
+        <v>273</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'KYCK') k, (</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'AUT1004') t</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'AUT1004');</v>
+      </c>
+      <c r="F73" t="s">
+        <v>163</v>
+      </c>
+      <c r="G73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>272</v>
+      </c>
+      <c r="B74" t="s">
+        <v>273</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO955') t</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO955');</v>
+      </c>
+      <c r="F74" t="s">
+        <v>165</v>
+      </c>
+      <c r="G74" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>272</v>
+      </c>
+      <c r="B75" t="s">
+        <v>273</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'KYK VSE') k, (</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN419') t</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN419');</v>
+      </c>
+      <c r="F75" t="s">
+        <v>167</v>
+      </c>
+      <c r="G75" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>272</v>
+      </c>
+      <c r="B76" t="s">
+        <v>273</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'TVSK') k, (</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN1260') t</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN1260');</v>
+      </c>
+      <c r="F76" t="s">
+        <v>170</v>
+      </c>
+      <c r="G76" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>272</v>
+      </c>
+      <c r="B77" t="s">
+        <v>273</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SCTWV ACHENSEE') k, (</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'AUT1178') t</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'AUT1178');</v>
+      </c>
+      <c r="F77" t="s">
+        <v>173</v>
+      </c>
+      <c r="G77" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>272</v>
+      </c>
+      <c r="B78" t="s">
+        <v>273</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK BURJA IZOLA') k, (</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO310') t</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO310');</v>
+      </c>
+      <c r="F78" t="s">
+        <v>175</v>
+      </c>
+      <c r="G78" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>272</v>
+      </c>
+      <c r="B79" t="s">
+        <v>273</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SMD PIRAN') k, (</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO849') t</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO849');</v>
+      </c>
+      <c r="F79" t="s">
+        <v>177</v>
+      </c>
+      <c r="G79" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>272</v>
+      </c>
+      <c r="B80" t="s">
+        <v>273</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK PIRAT') k, (</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO2112') t</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO2112');</v>
+      </c>
+      <c r="F80" t="s">
+        <v>178</v>
+      </c>
+      <c r="G80" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>272</v>
+      </c>
+      <c r="B81" t="s">
+        <v>273</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK LJUBLJANA') k, (</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO527') t</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO527');</v>
+      </c>
+      <c r="F81" t="s">
+        <v>180</v>
+      </c>
+      <c r="G81" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>272</v>
+      </c>
+      <c r="B82" t="s">
+        <v>273</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'TPK SIRENA') k, (</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA7707') t</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA7707');</v>
+      </c>
+      <c r="F82" t="s">
+        <v>181</v>
+      </c>
+      <c r="G82" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>272</v>
+      </c>
+      <c r="B83" t="s">
+        <v>273</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO958') t</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO958');</v>
+      </c>
+      <c r="F83" t="s">
+        <v>183</v>
+      </c>
+      <c r="G83" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>272</v>
+      </c>
+      <c r="B84" t="s">
+        <v>273</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BD RANCA PTUJ') k, (</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO729') t</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO729');</v>
+      </c>
+      <c r="F84" t="s">
+        <v>184</v>
+      </c>
+      <c r="G84" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>272</v>
+      </c>
+      <c r="B85" t="s">
+        <v>273</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'THE YKA') k, (</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'HUN378') t</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'HUN378');</v>
+      </c>
+      <c r="F85" t="s">
+        <v>187</v>
+      </c>
+      <c r="G85" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>272</v>
+      </c>
+      <c r="B86" t="s">
+        <v>273</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SVBG') k, (</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA7908') t</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA7908');</v>
+      </c>
+      <c r="F86" t="s">
+        <v>189</v>
+      </c>
+      <c r="G86" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>272</v>
+      </c>
+      <c r="B87" t="s">
+        <v>273</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BD RANCA PTUJ') k, (</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO724') t</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO724');</v>
+      </c>
+      <c r="F87" t="s">
+        <v>191</v>
+      </c>
+      <c r="G87" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>272</v>
+      </c>
+      <c r="B88" t="s">
+        <v>273</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SVBG') k, (</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA8388') t</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA8388');</v>
+      </c>
+      <c r="F88" t="s">
+        <v>193</v>
+      </c>
+      <c r="G88" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>272</v>
+      </c>
+      <c r="B89" t="s">
+        <v>273</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO911') t</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO911');</v>
+      </c>
+      <c r="F89" t="s">
+        <v>195</v>
+      </c>
+      <c r="G89" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>272</v>
+      </c>
+      <c r="B90" t="s">
+        <v>273</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK LJUBLJANA') k, (</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO821') t</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO821');</v>
+      </c>
+      <c r="F90" t="s">
+        <v>197</v>
+      </c>
+      <c r="G90" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>272</v>
+      </c>
+      <c r="B91" t="s">
+        <v>273</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SVBG') k, (</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA8886') t</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA8886');</v>
+      </c>
+      <c r="F91" t="s">
+        <v>198</v>
+      </c>
+      <c r="G91" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>272</v>
+      </c>
+      <c r="B92" t="s">
+        <v>273</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK BURJA IZOLA') k, (</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO368') t</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO368');</v>
+      </c>
+      <c r="F92" t="s">
+        <v>200</v>
+      </c>
+      <c r="G92" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>272</v>
+      </c>
+      <c r="B93" t="s">
+        <v>273</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO912') t</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO912');</v>
+      </c>
+      <c r="F93" t="s">
+        <v>202</v>
+      </c>
+      <c r="G93" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>272</v>
+      </c>
+      <c r="B94" t="s">
+        <v>273</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK PIRAT') k, (</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO188') t</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO188');</v>
+      </c>
+      <c r="F94" t="s">
+        <v>204</v>
+      </c>
+      <c r="G94" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>272</v>
+      </c>
+      <c r="B95" t="s">
+        <v>273</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'BD RANCA PTUJ') k, (</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO728') t</v>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO728');</v>
+      </c>
+      <c r="F95" t="s">
+        <v>205</v>
+      </c>
+      <c r="G95" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>272</v>
+      </c>
+      <c r="B96" t="s">
+        <v>273</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK PIRAT') k, (</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO759') t</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO759');</v>
+      </c>
+      <c r="F96" t="s">
+        <v>207</v>
+      </c>
+      <c r="G96" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>272</v>
+      </c>
+      <c r="B97" t="s">
+        <v>273</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK LJUBLJANA') k, (</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO587') t</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO587');</v>
+      </c>
+      <c r="F97" t="s">
+        <v>208</v>
+      </c>
+      <c r="G97" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>272</v>
+      </c>
+      <c r="B98" t="s">
+        <v>273</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SBSK') k, (</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SMR2') t</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SMR2');</v>
+      </c>
+      <c r="F98" t="s">
+        <v>210</v>
+      </c>
+      <c r="G98" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>272</v>
+      </c>
+      <c r="B99" t="s">
+        <v>273</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK BURJA IZOLA') k, (</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO37') t</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO37');</v>
+      </c>
+      <c r="F99" t="s">
+        <v>212</v>
+      </c>
+      <c r="G99" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>272</v>
+      </c>
+      <c r="B100" t="s">
+        <v>273</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK PIRAT') k, (</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO93') t</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO93');</v>
+      </c>
+      <c r="F100" t="s">
+        <v>214</v>
+      </c>
+      <c r="G100" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>272</v>
+      </c>
+      <c r="B101" t="s">
+        <v>273</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK BURJA IZOLA') k, (</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO393') t</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO393');</v>
+      </c>
+      <c r="F101" t="s">
+        <v>215</v>
+      </c>
+      <c r="G101" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>272</v>
+      </c>
+      <c r="B102" t="s">
+        <v>273</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'TPK SIRENA') k, (</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA8206') t</v>
+      </c>
+      <c r="E102" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA8206');</v>
+      </c>
+      <c r="F102" t="s">
+        <v>217</v>
+      </c>
+      <c r="G102" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>272</v>
+      </c>
+      <c r="B103" t="s">
+        <v>273</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK OLIMPIC') k, (</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO678') t</v>
+      </c>
+      <c r="E103" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO678');</v>
+      </c>
+      <c r="F103" t="s">
+        <v>219</v>
+      </c>
+      <c r="G103" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>272</v>
+      </c>
+      <c r="B104" t="s">
+        <v>273</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'TPK SIRENA') k, (</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA8581') t</v>
+      </c>
+      <c r="E104" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA8581');</v>
+      </c>
+      <c r="F104" t="s">
+        <v>221</v>
+      </c>
+      <c r="G104" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>272</v>
+      </c>
+      <c r="B105" t="s">
+        <v>273</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SVBG') k, (</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA4535') t</v>
+      </c>
+      <c r="E105" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA4535');</v>
+      </c>
+      <c r="F105" t="s">
+        <v>223</v>
+      </c>
+      <c r="G105" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>272</v>
+      </c>
+      <c r="B106" t="s">
+        <v>273</v>
+      </c>
+      <c r="C106" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK LJUBLJANA') k, (</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO526') t</v>
+      </c>
+      <c r="E106" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO526');</v>
+      </c>
+      <c r="F106" t="s">
+        <v>225</v>
+      </c>
+      <c r="G106" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>272</v>
+      </c>
+      <c r="B107" t="s">
+        <v>273</v>
+      </c>
+      <c r="C107" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SVBG') k, (</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA5') t</v>
+      </c>
+      <c r="E107" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA5');</v>
+      </c>
+      <c r="F107" t="s">
+        <v>227</v>
+      </c>
+      <c r="G107" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>272</v>
+      </c>
+      <c r="B108" t="s">
+        <v>273</v>
+      </c>
+      <c r="C108" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'TJ LANKROUN') k, (</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'CZE774') t</v>
+      </c>
+      <c r="E108" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'CZE774');</v>
+      </c>
+      <c r="F108" t="s">
+        <v>229</v>
+      </c>
+      <c r="G108" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>272</v>
+      </c>
+      <c r="B109" t="s">
+        <v>273</v>
+      </c>
+      <c r="C109" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK LJUBLJANA') k, (</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO855') t</v>
+      </c>
+      <c r="E109" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO855');</v>
+      </c>
+      <c r="F109" t="s">
+        <v>231</v>
+      </c>
+      <c r="G109" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>272</v>
+      </c>
+      <c r="B110" t="s">
+        <v>273</v>
+      </c>
+      <c r="C110" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO91') t</v>
+      </c>
+      <c r="E110" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO91');</v>
+      </c>
+      <c r="F110" t="s">
+        <v>233</v>
+      </c>
+      <c r="G110" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>272</v>
+      </c>
+      <c r="B111" t="s">
+        <v>273</v>
+      </c>
+      <c r="C111" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'SVBG') k, (</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'ITA111') t</v>
+      </c>
+      <c r="E111" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'ITA111');</v>
+      </c>
+      <c r="F111" t="s">
+        <v>234</v>
+      </c>
+      <c r="G111" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>272</v>
+      </c>
+      <c r="B112" t="s">
+        <v>273</v>
+      </c>
+      <c r="C112" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK BURJA IZOLA') k, (</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO373') t</v>
+      </c>
+      <c r="E112" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO373');</v>
+      </c>
+      <c r="F112" t="s">
+        <v>236</v>
+      </c>
+      <c r="G112" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>272</v>
+      </c>
+      <c r="B113" t="s">
+        <v>273</v>
+      </c>
+      <c r="C113" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'TVSK') k, (</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO1260') t</v>
+      </c>
+      <c r="E113" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO1260');</v>
+      </c>
+      <c r="F113" t="s">
+        <v>238</v>
+      </c>
+      <c r="G113" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>272</v>
+      </c>
+      <c r="B114" t="s">
+        <v>273</v>
+      </c>
+      <c r="C114" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO984') t</v>
+      </c>
+      <c r="E114" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO984');</v>
+      </c>
+      <c r="F114" t="s">
+        <v>239</v>
+      </c>
+      <c r="G114" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>272</v>
+      </c>
+      <c r="B115" t="s">
+        <v>273</v>
+      </c>
+      <c r="C115" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO611') t</v>
+      </c>
+      <c r="E115" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO611');</v>
+      </c>
+      <c r="F115" t="s">
+        <v>241</v>
+      </c>
+      <c r="G115" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>272</v>
+      </c>
+      <c r="B116" t="s">
+        <v>273</v>
+      </c>
+      <c r="C116" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO916') t</v>
+      </c>
+      <c r="E116" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO916');</v>
+      </c>
+      <c r="F116" t="s">
+        <v>243</v>
+      </c>
+      <c r="G116" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>272</v>
+      </c>
+      <c r="B117" t="s">
+        <v>273</v>
+      </c>
+      <c r="C117" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO962') t</v>
+      </c>
+      <c r="E117" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO962');</v>
+      </c>
+      <c r="F117" t="s">
+        <v>244</v>
+      </c>
+      <c r="G117" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>272</v>
+      </c>
+      <c r="B118" t="s">
+        <v>273</v>
+      </c>
+      <c r="C118" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D118" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO949') t</v>
+      </c>
+      <c r="E118" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO949');</v>
+      </c>
+      <c r="F118" t="s">
+        <v>246</v>
+      </c>
+      <c r="G118" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>272</v>
+      </c>
+      <c r="B119" t="s">
+        <v>273</v>
+      </c>
+      <c r="C119" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> SELECT idklub FROM klub WHERE ime = 'JK JADRO KOPER') k, (</v>
+      </c>
+      <c r="D119" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'SLO9') t</v>
+      </c>
+      <c r="E119" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec, sailno FROM clanstvo JOIN tekmovalec ON idtekmovalec = tekmovalec_idtekmovalec WHERE sailno = 'SLO9');</v>
+      </c>
+      <c r="F119" t="s">
+        <v>248</v>
+      </c>
+      <c r="G119" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>